<commit_message>
Actualización de Excel (Gestión de Sprints)
</commit_message>
<xml_diff>
--- a/Gestion/Gestion_Sprints.xlsx
+++ b/Gestion/Gestion_Sprints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="2" r:id="rId1"/>
@@ -667,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -793,6 +793,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1079,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K36"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,9 +1269,7 @@
         <v>44756</v>
       </c>
       <c r="D14" s="36"/>
-      <c r="E14" s="37">
-        <v>1</v>
-      </c>
+      <c r="E14" s="57"/>
       <c r="F14" s="51" t="s">
         <v>54</v>
       </c>
@@ -1709,7 +1708,7 @@
       <c r="B6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="58">
+      <c r="C6" s="59">
         <v>100</v>
       </c>
       <c r="D6" s="7">
@@ -1923,7 +1922,7 @@
       <c r="H23" s="15"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="57"/>
+      <c r="D26" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1970,7 +1969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Comenzada transición al nuevo proyecto
Tras decidir que el Inform LowCost no iba a ser "impactante", se ha decidido cambiar el projecto a un MindHive con nombre aún pendiente por decidir.
</commit_message>
<xml_diff>
--- a/Gestion/Gestion_Sprints.xlsx
+++ b/Gestion/Gestion_Sprints.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5851C4EB-955F-436F-A655-F25FA7CA5265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5745" yWindow="135" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="2" r:id="rId1"/>
@@ -153,9 +154,6 @@
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Realizar primer montaje y comprobar que todo funcione</t>
-  </si>
-  <si>
     <t>Sprint 4</t>
   </si>
   <si>
@@ -168,9 +166,6 @@
     <t>Montaje de PCB</t>
   </si>
   <si>
-    <t>Realizar Simulador Unity</t>
-  </si>
-  <si>
     <t>Montar Red Neuronal para generar mapa de profundidades</t>
   </si>
   <si>
@@ -223,12 +218,18 @@
   </si>
   <si>
     <t>Debido al alto número de I/O necesario, se van a utilizar Shift Registers para ampliar el I/O del MCU. En concreto se van a usar 74hc595 (SIPO) y 74hc165 (PISO)</t>
+  </si>
+  <si>
+    <t>Realizar Simulador en Unity</t>
+  </si>
+  <si>
+    <t>Realizar primer montaje (Breadboard) y comprobar que todo funcione</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -717,9 +718,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -736,67 +734,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="39"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="39"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="39"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="39"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="39"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="39"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1077,11 +1078,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,11 +1095,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="16" t="s">
         <v>31</v>
       </c>
@@ -1119,10 +1120,10 @@
       <c r="K3" s="20"/>
     </row>
     <row r="4" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="58"/>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
@@ -1133,101 +1134,101 @@
       <c r="K4" s="20"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="25"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24"/>
     </row>
     <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="56"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="48"/>
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="48"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="56"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="48"/>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="48"/>
     </row>
     <row r="10" spans="2:11" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="44"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
@@ -1238,316 +1239,312 @@
       <c r="K12" s="20"/>
     </row>
     <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="23" t="s">
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="22" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="36">
+      <c r="B14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="35">
         <v>44756</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="37"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="36"/>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C15" s="35">
         <v>44773</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="51" t="s">
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="37"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="36"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="36">
+      <c r="C16" s="35">
         <v>44787</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="51" t="s">
+      <c r="D16" s="35"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="37"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="36"/>
     </row>
     <row r="17" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="36">
+      <c r="C17" s="35">
         <v>44794</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="51" t="s">
+      <c r="D17" s="35"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="36"/>
+    </row>
+    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="37"/>
-    </row>
-    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="35" t="s">
+      <c r="C18" s="35">
+        <v>44798</v>
+      </c>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="36">
-        <v>44798</v>
-      </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="51" t="s">
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="36"/>
+    </row>
+    <row r="19" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="37"/>
-    </row>
-    <row r="19" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="35" t="s">
+      <c r="C19" s="35">
+        <v>44815</v>
+      </c>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="36">
-        <v>44815</v>
-      </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="51" t="s">
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="36"/>
+    </row>
+    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="35">
+        <v>44829</v>
+      </c>
+      <c r="D20" s="35"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="36"/>
+    </row>
+    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="35">
+        <v>44836</v>
+      </c>
+      <c r="D21" s="35"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="37"/>
-    </row>
-    <row r="20" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="35" t="s">
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="36"/>
+    </row>
+    <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="36">
-        <v>44829</v>
-      </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="37"/>
-    </row>
-    <row r="21" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="35" t="s">
+      <c r="C22" s="35">
+        <v>44850</v>
+      </c>
+      <c r="D22" s="35"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="36">
-        <v>44836</v>
-      </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="37"/>
-    </row>
-    <row r="22" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="36">
-        <v>44850</v>
-      </c>
-      <c r="D22" s="36"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="37"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="36"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="37"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="36"/>
     </row>
     <row r="28" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="44"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="41"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="54"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="47"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="57"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="45" t="s">
+      <c r="B32" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="47"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="57"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="47"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="57"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="47"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="57"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="46"/>
-      <c r="K35" s="47"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="57"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="48"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="50"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F23:J23"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="F22:J22"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="B36:K36"/>
     <mergeCell ref="F14:J14"/>
     <mergeCell ref="F15:J15"/>
@@ -1564,9 +1561,13 @@
     <mergeCell ref="B32:K32"/>
     <mergeCell ref="B33:K33"/>
     <mergeCell ref="B34:K34"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F23:J23"/>
+    <mergeCell ref="F17:J17"/>
+    <mergeCell ref="F18:J18"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="F20:J20"/>
+    <mergeCell ref="F21:J21"/>
+    <mergeCell ref="F22:J22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1574,7 +1575,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -1634,7 +1635,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3" s="7">
         <v>100</v>
@@ -1650,7 +1651,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1658,7 +1659,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" s="7">
         <v>100</v>
@@ -1674,7 +1675,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1682,7 +1683,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="7">
         <v>100</v>
@@ -1698,7 +1699,7 @@
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1706,9 +1707,9 @@
         <v>12</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="59">
+        <v>57</v>
+      </c>
+      <c r="C6" s="39">
         <v>100</v>
       </c>
       <c r="D6" s="7">
@@ -1722,7 +1723,7 @@
         <v>9</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1730,7 +1731,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" s="7">
         <v>90</v>
@@ -1752,7 +1753,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8" s="7">
         <v>95</v>
@@ -1768,7 +1769,7 @@
         <v>9</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1922,7 +1923,7 @@
       <c r="H23" s="15"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D26" s="58"/>
+      <c r="D26" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1930,7 +1931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1942,7 +1943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1954,7 +1955,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1966,7 +1967,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1980,7 +1981,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>